<commit_message>
React Minor Issue solved
</commit_message>
<xml_diff>
--- a/E-Pariksha/Testcase.xlsx
+++ b/E-Pariksha/Testcase.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="178">
   <si>
     <t>Process</t>
   </si>
@@ -101,9 +101,6 @@
     <t>login success</t>
   </si>
   <si>
-    <t>wrong place holder at email textbox</t>
-  </si>
-  <si>
     <t>http://localhost:8081/teacher_login</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Teacher login page loading</t>
   </si>
   <si>
-    <t>http://localhost:8081/student_login</t>
-  </si>
-  <si>
     <t>Student login page loading</t>
   </si>
   <si>
@@ -167,9 +161,6 @@
     <t>Pending</t>
   </si>
   <si>
-    <t>New student add pending</t>
-  </si>
-  <si>
     <t>Success</t>
   </si>
   <si>
@@ -194,9 +185,6 @@
     <t>Interface to add new teacher and its credentials</t>
   </si>
   <si>
-    <t>Actual data in reports pending</t>
-  </si>
-  <si>
     <t>http://localhost:8081/admin/subject</t>
   </si>
   <si>
@@ -230,15 +218,6 @@
     <t>Subject add successful</t>
   </si>
   <si>
-    <t>http://localhost:8081/admin/user-profile</t>
-  </si>
-  <si>
-    <t>Admin profile information</t>
-  </si>
-  <si>
-    <t>Display profile information of admin</t>
-  </si>
-  <si>
     <t>http://localhost:8081/admin/logout</t>
   </si>
   <si>
@@ -248,9 +227,6 @@
     <t>Admin logout to index page</t>
   </si>
   <si>
-    <t>Display admin information</t>
-  </si>
-  <si>
     <t>Admin logout to index.html successfully</t>
   </si>
   <si>
@@ -413,9 +389,6 @@
     <t>Display exam information</t>
   </si>
   <si>
-    <t>Actual data not receving</t>
-  </si>
-  <si>
     <t>http://localhost:8081/admin/exam_add</t>
   </si>
   <si>
@@ -428,9 +401,6 @@
     <t>Assign new exam set</t>
   </si>
   <si>
-    <t>Actual Assign pending</t>
-  </si>
-  <si>
     <t>http://localhost:8081/admin/question</t>
   </si>
   <si>
@@ -443,9 +413,6 @@
     <t>Display questionkeys</t>
   </si>
   <si>
-    <t>Actual questions insert pending</t>
-  </si>
-  <si>
     <t>http://localhost:8081/admin/exam_history</t>
   </si>
   <si>
@@ -489,6 +456,111 @@
   </si>
   <si>
     <t>Display teacher profile</t>
+  </si>
+  <si>
+    <t>http://localhost:3000</t>
+  </si>
+  <si>
+    <t>report with actual data</t>
+  </si>
+  <si>
+    <t>Assign new exam success</t>
+  </si>
+  <si>
+    <t>Actual questions insert successful</t>
+  </si>
+  <si>
+    <t>Exam history unsuccessfull</t>
+  </si>
+  <si>
+    <t>Result displayed</t>
+  </si>
+  <si>
+    <t>Display information regarding exam</t>
+  </si>
+  <si>
+    <t>Exam data</t>
+  </si>
+  <si>
+    <t>Teacher profile info</t>
+  </si>
+  <si>
+    <t>Actual data in reports Working</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/dashboard</t>
+  </si>
+  <si>
+    <t>Start exam and upcoming exam info</t>
+  </si>
+  <si>
+    <t>Dashboard with start exam button</t>
+  </si>
+  <si>
+    <t>Add Exam to students</t>
+  </si>
+  <si>
+    <t>Add new exam</t>
+  </si>
+  <si>
+    <t>Assign exam</t>
+  </si>
+  <si>
+    <t>Result view to teacher</t>
+  </si>
+  <si>
+    <t>Display result to teacher</t>
+  </si>
+  <si>
+    <t>unsuccesss</t>
+  </si>
+  <si>
+    <t>Result report</t>
+  </si>
+  <si>
+    <t>Exam history report</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>Dashboard view</t>
+  </si>
+  <si>
+    <t>Instant result</t>
+  </si>
+  <si>
+    <t>exam history info</t>
+  </si>
+  <si>
+    <t>unsuccess</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/Start</t>
+  </si>
+  <si>
+    <t>Instruction page with start exam button</t>
+  </si>
+  <si>
+    <t>Start exam</t>
+  </si>
+  <si>
+    <t>Instruction view</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/Exam</t>
+  </si>
+  <si>
+    <t>Actual Exam Portal-E-Parikhsha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-Parikhsha exam </t>
+  </si>
+  <si>
+    <t>Exam page</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/result</t>
   </si>
 </sst>
 </file>
@@ -635,7 +707,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -643,6 +714,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -668,13 +742,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1000,7 +1074,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1008,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J105"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="15"/>
@@ -1073,16 +1147,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="12">
         <v>1</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1094,13 +1168,13 @@
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="I6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J6" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1108,22 +1182,22 @@
         <v>2</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1137,16 +1211,16 @@
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="I10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16.899999999999999" customHeight="1">
@@ -1154,10 +1228,10 @@
         <v>4</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F12" t="s">
         <v>18</v>
@@ -1166,10 +1240,10 @@
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="I12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="17.45" customHeight="1"/>
@@ -1178,22 +1252,22 @@
         <v>5</v>
       </c>
       <c r="D14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
         <v>80</v>
       </c>
-      <c r="E14" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" t="s">
-        <v>88</v>
-      </c>
       <c r="I14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1201,27 +1275,27 @@
         <v>6</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="I16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>19</v>
@@ -1230,13 +1304,13 @@
         <v>1</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F22" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>12</v>
@@ -1259,13 +1333,13 @@
         <v>2</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>12</v>
@@ -1276,28 +1350,28 @@
       <c r="I23" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>24</v>
+      <c r="J23" s="16" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="6">
         <v>1</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F28" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>12</v>
@@ -1309,61 +1383,61 @@
         <v>15</v>
       </c>
       <c r="J28" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="20" t="s">
-        <v>104</v>
+      <c r="A29" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C29" s="6">
         <v>2</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E29" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F29" t="s">
-        <v>98</v>
-      </c>
-      <c r="G29" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H29" t="s">
         <v>23</v>
       </c>
       <c r="I29" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J29" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="B30" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>28</v>
+        <v>143</v>
       </c>
       <c r="C36" s="6">
         <v>1</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E36" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F36" t="s">
         <v>20</v>
@@ -1375,622 +1449,783 @@
         <v>14</v>
       </c>
       <c r="I36" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J36" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="20" t="s">
-        <v>104</v>
+      <c r="A37" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C37" s="6">
         <v>2</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F37" t="s">
-        <v>98</v>
-      </c>
-      <c r="G37" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G37" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I37" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="B38" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C46" s="6">
         <v>1</v>
       </c>
       <c r="D46" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" t="s">
         <v>38</v>
       </c>
-      <c r="E46" t="s">
-        <v>40</v>
-      </c>
       <c r="F46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H46" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I46" t="s">
-        <v>47</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
+      </c>
+      <c r="J46" s="16" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="B48" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C48" s="6">
         <v>2</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E48" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F48" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H48" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="I48" t="s">
-        <v>47</v>
-      </c>
-      <c r="J48" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="J48" s="16" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="2:10">
       <c r="B50" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C50" s="6">
         <v>3</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F50" t="s">
+        <v>61</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" t="s">
+        <v>60</v>
+      </c>
+      <c r="I50" t="s">
         <v>43</v>
       </c>
-      <c r="G50" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="H50" t="s">
-        <v>64</v>
-      </c>
-      <c r="I50" t="s">
-        <v>45</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>46</v>
+      <c r="J50" s="16" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="2:10">
       <c r="B52" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C52" s="6">
         <v>4</v>
       </c>
       <c r="D52" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E52" t="s">
         <v>50</v>
       </c>
-      <c r="E52" t="s">
-        <v>53</v>
-      </c>
       <c r="F52" t="s">
-        <v>111</v>
-      </c>
-      <c r="G52" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G52" s="17" t="s">
         <v>12</v>
       </c>
       <c r="H52" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="I52" t="s">
-        <v>47</v>
-      </c>
-      <c r="J52" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="J52" s="16" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="2:10">
       <c r="B54" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C54" s="6">
         <v>5</v>
       </c>
       <c r="D54" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" t="s">
         <v>51</v>
       </c>
-      <c r="E54" t="s">
-        <v>54</v>
-      </c>
       <c r="F54" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G54" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H54" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I54" t="s">
-        <v>47</v>
-      </c>
-      <c r="J54" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="J54" s="16" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="2:10">
       <c r="B56" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C56" s="6">
         <v>6</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E56" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F56" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G56" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H56" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="I56" t="s">
-        <v>47</v>
-      </c>
-      <c r="J56" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="J56" s="16" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="2:10">
       <c r="B58" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C58" s="6">
         <v>7</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E58" t="s">
+        <v>57</v>
+      </c>
+      <c r="F58" t="s">
         <v>61</v>
       </c>
-      <c r="F58" t="s">
-        <v>65</v>
-      </c>
       <c r="G58" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H58" t="s">
+        <v>58</v>
+      </c>
+      <c r="I58" t="s">
+        <v>44</v>
+      </c>
+      <c r="J58" s="16" t="s">
         <v>62</v>
-      </c>
-      <c r="I58" t="s">
-        <v>47</v>
-      </c>
-      <c r="J58" s="17" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="60" spans="2:10">
       <c r="B60" s="5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C60" s="6">
         <v>8</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E60" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F60" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H60" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="I60" t="s">
-        <v>47</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>128</v>
+        <v>44</v>
+      </c>
+      <c r="J60" s="16" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="2:10">
       <c r="B62" s="5" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C62" s="6">
         <v>9</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E62" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F62" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H62" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="I62" t="s">
-        <v>47</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>133</v>
+        <v>44</v>
+      </c>
+      <c r="J62" s="16" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="64" spans="2:10">
       <c r="B64" s="5" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C64" s="6">
         <v>10</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E64" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F64" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H64" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="I64" t="s">
-        <v>47</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>138</v>
+        <v>44</v>
+      </c>
+      <c r="J64" s="16" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="B66" s="5" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C66" s="6">
         <v>11</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E66" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="F66" t="s">
+        <v>41</v>
+      </c>
+      <c r="G66" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G66" s="14" t="s">
-        <v>45</v>
+      <c r="H66" t="s">
+        <v>163</v>
+      </c>
+      <c r="I66" t="s">
+        <v>43</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="B68" s="5" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C68" s="6">
         <v>12</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E68" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="F68" t="s">
-        <v>43</v>
-      </c>
-      <c r="G68" s="14" t="s">
-        <v>45</v>
+        <v>41</v>
+      </c>
+      <c r="G68" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68" t="s">
+        <v>148</v>
+      </c>
+      <c r="I68" t="s">
+        <v>44</v>
+      </c>
+      <c r="J68" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="B70" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C70" s="6">
         <v>13</v>
       </c>
       <c r="D70" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E70" t="s">
+        <v>65</v>
+      </c>
+      <c r="F70" t="s">
+        <v>61</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70" t="s">
+        <v>64</v>
+      </c>
+      <c r="I70" t="s">
+        <v>44</v>
+      </c>
+      <c r="J70" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" t="s">
+        <v>114</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C76" s="6">
+        <v>1</v>
+      </c>
+      <c r="D76" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E76" t="s">
+        <v>37</v>
+      </c>
+      <c r="F76" t="s">
+        <v>61</v>
+      </c>
+      <c r="G76" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H76" t="s">
         <v>69</v>
       </c>
-      <c r="F70" t="s">
-        <v>65</v>
-      </c>
-      <c r="G70" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H70" t="s">
-        <v>73</v>
-      </c>
-      <c r="I70" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10">
-      <c r="B72" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C72" s="6">
-        <v>14</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E72" t="s">
-        <v>72</v>
-      </c>
-      <c r="F72" t="s">
-        <v>65</v>
-      </c>
-      <c r="G72" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H72" t="s">
-        <v>71</v>
-      </c>
-      <c r="I72" t="s">
-        <v>47</v>
-      </c>
-      <c r="J72" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
-      <c r="A77" t="s">
-        <v>122</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C77" s="6">
+      <c r="I76" t="s">
+        <v>44</v>
+      </c>
+      <c r="J76" s="16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="B78" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C78" s="6">
+        <v>2</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E78" t="s">
+        <v>49</v>
+      </c>
+      <c r="F78" t="s">
+        <v>102</v>
+      </c>
+      <c r="G78" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H78" t="s">
+        <v>42</v>
+      </c>
+      <c r="I78" t="s">
+        <v>44</v>
+      </c>
+      <c r="J78" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="B80" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C80" s="6">
+        <v>3</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F80" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G80" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="I80" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="J80" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10">
+      <c r="B82" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C82" s="6">
+        <v>4</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E82" t="s">
+        <v>157</v>
+      </c>
+      <c r="F82" t="s">
+        <v>61</v>
+      </c>
+      <c r="G82" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H82" t="s">
+        <v>158</v>
+      </c>
+      <c r="I82" t="s">
+        <v>44</v>
+      </c>
+      <c r="J82" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10">
+      <c r="B84" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C84" s="6">
+        <v>5</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E84" t="s">
+        <v>138</v>
+      </c>
+      <c r="F84" t="s">
+        <v>139</v>
+      </c>
+      <c r="G84" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H84" t="s">
+        <v>140</v>
+      </c>
+      <c r="I84" t="s">
+        <v>44</v>
+      </c>
+      <c r="J84" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="86" spans="2:10">
+      <c r="B86" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C86" s="6">
+        <v>6</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E86" t="s">
+        <v>160</v>
+      </c>
+      <c r="F86" t="s">
+        <v>84</v>
+      </c>
+      <c r="G86" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H86" t="s">
+        <v>162</v>
+      </c>
+      <c r="I86" t="s">
+        <v>161</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="88" spans="2:10">
+      <c r="B88" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C88" s="6">
+        <v>7</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E88" t="s">
+        <v>142</v>
+      </c>
+      <c r="F88" t="s">
+        <v>61</v>
+      </c>
+      <c r="G88" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H88" t="s">
+        <v>151</v>
+      </c>
+      <c r="I88" t="s">
+        <v>15</v>
+      </c>
+      <c r="J88" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="2:10">
+      <c r="C90" s="6">
+        <v>8</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" t="s">
+        <v>115</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C100" s="6">
         <v>1</v>
       </c>
-      <c r="D77" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E77" t="s">
-        <v>39</v>
-      </c>
-      <c r="F77" t="s">
-        <v>65</v>
-      </c>
-      <c r="G77" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H77" t="s">
-        <v>77</v>
-      </c>
-      <c r="I77" t="s">
-        <v>47</v>
-      </c>
-      <c r="J77" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
-      <c r="B79" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C79" s="6">
+      <c r="D100" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E100" t="s">
+        <v>155</v>
+      </c>
+      <c r="F100" t="s">
+        <v>61</v>
+      </c>
+      <c r="G100" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H100" t="s">
+        <v>165</v>
+      </c>
+      <c r="I100" t="s">
+        <v>15</v>
+      </c>
+      <c r="J100" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="B102" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C102" s="6">
         <v>2</v>
       </c>
-      <c r="D79" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E79" t="s">
-        <v>52</v>
-      </c>
-      <c r="F79" t="s">
-        <v>110</v>
-      </c>
-      <c r="G79" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H79" t="s">
-        <v>44</v>
-      </c>
-      <c r="I79" t="s">
-        <v>47</v>
-      </c>
-      <c r="J79" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="81" spans="2:10">
-      <c r="B81" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C81" s="6">
+      <c r="D102" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E102" t="s">
+        <v>171</v>
+      </c>
+      <c r="F102" t="s">
+        <v>61</v>
+      </c>
+      <c r="G102" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H102" t="s">
+        <v>172</v>
+      </c>
+      <c r="I102" t="s">
+        <v>15</v>
+      </c>
+      <c r="J102" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="B104" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C104" s="6">
         <v>3</v>
       </c>
-      <c r="G81" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="83" spans="2:10">
-      <c r="B83" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C83" s="6">
+      <c r="D104" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E104" t="s">
+        <v>175</v>
+      </c>
+      <c r="F104" t="s">
+        <v>61</v>
+      </c>
+      <c r="G104" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H104" t="s">
+        <v>176</v>
+      </c>
+      <c r="I104" t="s">
+        <v>15</v>
+      </c>
+      <c r="J104" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="B106" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C106" s="6">
         <v>4</v>
       </c>
-      <c r="G83" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="85" spans="2:10">
-      <c r="B85" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C85" s="6">
+      <c r="D106" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E106" t="s">
+        <v>83</v>
+      </c>
+      <c r="F106" t="s">
+        <v>61</v>
+      </c>
+      <c r="G106" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H106" t="s">
+        <v>166</v>
+      </c>
+      <c r="I106" t="s">
+        <v>15</v>
+      </c>
+      <c r="J106" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="C108" s="6">
         <v>5</v>
       </c>
-      <c r="D85" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E85" t="s">
-        <v>149</v>
-      </c>
-      <c r="F85" t="s">
-        <v>150</v>
-      </c>
-      <c r="G85" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H85" t="s">
-        <v>151</v>
-      </c>
-      <c r="I85" t="s">
-        <v>47</v>
-      </c>
-      <c r="J85" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="87" spans="2:10">
-      <c r="B87" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C87" s="6">
-        <v>6</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G87" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="89" spans="2:10">
-      <c r="B89" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C89" s="6">
-        <v>7</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E89" t="s">
-        <v>153</v>
-      </c>
-      <c r="G89" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="91" spans="2:10">
-      <c r="C91" s="6">
-        <v>8</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7">
-      <c r="A101" t="s">
-        <v>123</v>
-      </c>
-      <c r="C101" s="6">
-        <v>1</v>
-      </c>
-      <c r="G101" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7">
-      <c r="C103" s="6">
-        <v>2</v>
-      </c>
-      <c r="D103" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E103" t="s">
-        <v>91</v>
-      </c>
-      <c r="F103" t="s">
-        <v>92</v>
-      </c>
-      <c r="G103" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7">
-      <c r="C105" s="6">
-        <v>3</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G105" s="14" t="s">
-        <v>45</v>
+      <c r="D108" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E108" t="s">
+        <v>163</v>
+      </c>
+      <c r="F108" t="s">
+        <v>41</v>
+      </c>
+      <c r="G108" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H108" t="s">
+        <v>167</v>
+      </c>
+      <c r="I108" t="s">
+        <v>168</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2006,23 +2241,26 @@
     <hyperlink ref="B54" r:id="rId9"/>
     <hyperlink ref="B56" r:id="rId10"/>
     <hyperlink ref="B58" r:id="rId11"/>
-    <hyperlink ref="B70" r:id="rId12"/>
-    <hyperlink ref="B72" r:id="rId13"/>
-    <hyperlink ref="B77" r:id="rId14"/>
-    <hyperlink ref="B79" r:id="rId15"/>
-    <hyperlink ref="B81" r:id="rId16"/>
-    <hyperlink ref="B83" r:id="rId17"/>
-    <hyperlink ref="B85" r:id="rId18"/>
-    <hyperlink ref="B87" r:id="rId19"/>
-    <hyperlink ref="B89" r:id="rId20"/>
-    <hyperlink ref="B60" r:id="rId21"/>
-    <hyperlink ref="B62" r:id="rId22"/>
-    <hyperlink ref="B64" r:id="rId23"/>
-    <hyperlink ref="B66" r:id="rId24"/>
-    <hyperlink ref="B68" r:id="rId25"/>
+    <hyperlink ref="B76" r:id="rId12"/>
+    <hyperlink ref="B78" r:id="rId13"/>
+    <hyperlink ref="B80" r:id="rId14"/>
+    <hyperlink ref="B82" r:id="rId15"/>
+    <hyperlink ref="B84" r:id="rId16"/>
+    <hyperlink ref="B86" r:id="rId17"/>
+    <hyperlink ref="B88" r:id="rId18"/>
+    <hyperlink ref="B60" r:id="rId19"/>
+    <hyperlink ref="B62" r:id="rId20"/>
+    <hyperlink ref="B64" r:id="rId21"/>
+    <hyperlink ref="B66" r:id="rId22"/>
+    <hyperlink ref="B68" r:id="rId23"/>
+    <hyperlink ref="B70" r:id="rId24"/>
+    <hyperlink ref="B100" r:id="rId25"/>
+    <hyperlink ref="B102" r:id="rId26"/>
+    <hyperlink ref="B104" r:id="rId27"/>
+    <hyperlink ref="B106" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId26"/>
-  <drawing r:id="rId27"/>
+  <pageSetup orientation="portrait" r:id="rId29"/>
+  <drawing r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>